<commit_message>
Add colorization to excel sheet
</commit_message>
<xml_diff>
--- a/Entropie.xlsx
+++ b/Entropie.xlsx
@@ -1,36 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29010"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://seagullbird-my.sharepoint.com/personal/michael_vogler_seagullbird_ch/Documents/Schule/HSLU/Technik/Tag2_GrundlagenComputersicherheit/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="11_AD4DB114E441178AC67DF4407613C4B8693EDF10" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9664CDB-9BE3-4BF7-A93A-033E21AEC10C}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="16236" yWindow="4764" windowWidth="27156" windowHeight="19272" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Entropie" sheetId="1" r:id="rId1"/>
-    <sheet name="Bell-LaPadula" sheetId="2" r:id="rId2"/>
+    <sheet name="Entropie" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Bell-LaPadula" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -42,68 +26,107 @@
     <t xml:space="preserve">Zeichensatz A </t>
   </si>
   <si>
-    <t>Klein (äöü)</t>
-  </si>
-  <si>
-    <t>gross (äöü)</t>
-  </si>
-  <si>
-    <t>Ziffern</t>
-  </si>
-  <si>
-    <t>Zeichen</t>
+    <t xml:space="preserve">Klein (äöü)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gross (äöü)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ziffern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zeichen</t>
   </si>
   <si>
     <t xml:space="preserve">Zeichensatz B </t>
   </si>
   <si>
-    <t>Sonderzeichen</t>
-  </si>
-  <si>
-    <t>Anzahl Zeichen</t>
-  </si>
-  <si>
-    <t>Mögliche Zeichen</t>
-  </si>
-  <si>
-    <t>Entropie pro Zeichen - log_2(Mögliche Zeichen)</t>
-  </si>
-  <si>
-    <t>Entropie Gesamt - Anzahl Zeichen*Entropie</t>
-  </si>
-  <si>
-    <t>Anzahl Kombinationen - Mögliche Zeichen^Anzahl</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
+    <t xml:space="preserve">Sonderzeichen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anzahl Zeichen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mögliche Zeichen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entropie pro Zeichen - log_2(Mögliche Zeichen)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entropie Gesamt - Anzahl Zeichen*Entropie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anzahl Kombinationen - Mögliche Zeichen^Anzahl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.00E+00"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8F2A1"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFB66C"/>
+        <bgColor rgb="FFFF99CC"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -111,185 +134,220 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="6">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFE8F2A1"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFB66C"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="44546a"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="e7e6e6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="5b9bd5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="ed7d31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="a5a5a5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="ffc000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4472c4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="70ad47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0563c1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="954f72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme>
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
                 <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
                 <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
                 <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
                 <a:lumMod val="102000"/>
                 <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
                 <a:lumMod val="100000"/>
                 <a:shade val="100000"/>
               </a:schemeClr>
@@ -297,33 +355,24 @@
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
                 <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
@@ -336,13 +385,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -352,15 +395,13 @@
         <a:solidFill>
           <a:schemeClr val="phClr">
             <a:tint val="95000"/>
-            <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="93000"/>
-                <a:satMod val="150000"/>
                 <a:shade val="98000"/>
                 <a:lumMod val="102000"/>
               </a:schemeClr>
@@ -368,7 +409,6 @@
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:tint val="98000"/>
-                <a:satMod val="130000"/>
                 <a:shade val="90000"/>
                 <a:lumMod val="103000"/>
               </a:schemeClr>
@@ -376,179 +416,201 @@
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="63000"/>
-                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:G14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="39.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="36.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" t="s">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="1" t="n">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
-      <c r="B2" t="s">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1" t="n">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
-      <c r="B3" t="s">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
-      <c r="B4" t="s">
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
-      <c r="A6" t="s">
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1" t="n">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
-      <c r="B7" t="s">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
-      <c r="B13" t="s">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
-      <c r="A14" t="s">
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C14">
-        <f>SUM(C1:C4)</f>
+      <c r="C14" s="2" t="n">
+        <f aca="false">SUM(C1:C4)</f>
         <v>62</v>
       </c>
-      <c r="E14">
-        <f>LOG(C14,2)</f>
-        <v>5.9541963103868758</v>
-      </c>
-      <c r="G14">
-        <f>B14*E14</f>
-        <v>47.633570483095006</v>
-      </c>
-      <c r="I14">
-        <f>C14^B14</f>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="n">
+        <f aca="false">LOG(C14,2)</f>
+        <v>5.95419631038688</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="3" t="n">
+        <f aca="false">B14*E14</f>
+        <v>47.633570483095</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="4" t="n">
+        <f aca="false">C14^B14</f>
         <v>218340105584896</v>
       </c>
-      <c r="L14" s="1"/>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" t="s">
+      <c r="L14" s="5"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="C15">
-        <f>SUM(C6:C7)</f>
+      <c r="C15" s="2" t="n">
+        <f aca="false">SUM(C6:C7)</f>
         <v>32</v>
       </c>
-      <c r="E15">
-        <f>LOG(C15,2)</f>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="n">
+        <f aca="false">LOG(C15,2)</f>
         <v>5</v>
       </c>
-      <c r="G15">
-        <f>B15*E15</f>
+      <c r="F15" s="2"/>
+      <c r="G15" s="3" t="n">
+        <f aca="false">B15*E15</f>
         <v>35</v>
       </c>
-      <c r="I15">
-        <f>C15^B15</f>
+      <c r="H15" s="2"/>
+      <c r="I15" s="4" t="n">
+        <f aca="false">C15^B15</f>
         <v>34359738368</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E0BAFB-462D-4B8C-9405-2E74D8209522}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fix titles to be easily understandable
</commit_message>
<xml_diff>
--- a/Entropie.xlsx
+++ b/Entropie.xlsx
@@ -50,13 +50,13 @@
     <t xml:space="preserve">Mögliche Zeichen</t>
   </si>
   <si>
-    <t xml:space="preserve">Entropie pro Zeichen - log_2(Mögliche Zeichen)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entropie Gesamt - Anzahl Zeichen*Entropie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anzahl Kombinationen - Mögliche Zeichen^Anzahl</t>
+    <t xml:space="preserve">Entropie pro Zeichen: log_2(Mögliche Zeichen)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entropie Gesamt: Anzahl Zeichen*Entropie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anzahl Kombinationen: Mögliche Zeichen^Anzahl</t>
   </si>
   <si>
     <t xml:space="preserve">A</t>
@@ -159,28 +159,32 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -436,146 +440,146 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="39.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="36.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="39.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="36.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="C1" s="2" t="n">
         <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C2" s="2" t="n">
         <v>26</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="2" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="1"/>
+      <c r="C5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="2" t="n">
         <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="C7" s="2" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="0" t="s">
+      <c r="G13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="0" t="s">
+      <c r="I13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="1" t="n">
+      <c r="B14" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="C14" s="2" t="n">
+      <c r="C14" s="3" t="n">
         <f aca="false">SUM(C1:C4)</f>
         <v>62</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2" t="n">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3" t="n">
         <f aca="false">LOG(C14,2)</f>
         <v>5.95419631038688</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="3" t="n">
+      <c r="F14" s="3"/>
+      <c r="G14" s="4" t="n">
         <f aca="false">B14*E14</f>
         <v>47.633570483095</v>
       </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="4" t="n">
+      <c r="H14" s="3"/>
+      <c r="I14" s="5" t="n">
         <f aca="false">C14^B14</f>
         <v>218340105584896</v>
       </c>
-      <c r="L14" s="5"/>
+      <c r="L14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="1" t="n">
+      <c r="B15" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="C15" s="2" t="n">
+      <c r="C15" s="3" t="n">
         <f aca="false">SUM(C6:C7)</f>
         <v>32</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2" t="n">
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="n">
         <f aca="false">LOG(C15,2)</f>
         <v>5</v>
       </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="3" t="n">
+      <c r="F15" s="3"/>
+      <c r="G15" s="4" t="n">
         <f aca="false">B15*E15</f>
         <v>35</v>
       </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="4" t="n">
+      <c r="H15" s="3"/>
+      <c r="I15" s="5" t="n">
         <f aca="false">C15^B15</f>
         <v>34359738368</v>
       </c>

</xml_diff>

<commit_message>
Fix titles to be fat
</commit_message>
<xml_diff>
--- a/Entropie.xlsx
+++ b/Entropie.xlsx
@@ -159,7 +159,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -168,7 +168,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -440,14 +448,14 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="39.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="36.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="42"/>
@@ -456,130 +464,139 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="n">
+      <c r="C1" s="3" t="n">
         <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="3" t="n">
         <v>26</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="3" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1" t="s">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="2"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" s="3" t="n">
         <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="1" t="s">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C7" s="3" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="D13" s="4"/>
+      <c r="E13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="F13" s="4"/>
+      <c r="G13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="H13" s="4"/>
+      <c r="I13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="2" t="n">
+      <c r="B14" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="C14" s="3" t="n">
+      <c r="C14" s="5" t="n">
         <f aca="false">SUM(C1:C4)</f>
         <v>62</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3" t="n">
+      <c r="D14" s="5"/>
+      <c r="E14" s="5" t="n">
         <f aca="false">LOG(C14,2)</f>
         <v>5.95419631038688</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="4" t="n">
+      <c r="F14" s="5"/>
+      <c r="G14" s="6" t="n">
         <f aca="false">B14*E14</f>
         <v>47.633570483095</v>
       </c>
-      <c r="H14" s="3"/>
-      <c r="I14" s="5" t="n">
+      <c r="H14" s="5"/>
+      <c r="I14" s="7" t="n">
         <f aca="false">C14^B14</f>
         <v>218340105584896</v>
       </c>
-      <c r="L14" s="6"/>
+      <c r="L14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="2" t="n">
+      <c r="B15" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="C15" s="3" t="n">
+      <c r="C15" s="5" t="n">
         <f aca="false">SUM(C6:C7)</f>
         <v>32</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3" t="n">
+      <c r="D15" s="5"/>
+      <c r="E15" s="5" t="n">
         <f aca="false">LOG(C15,2)</f>
         <v>5</v>
       </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="4" t="n">
+      <c r="F15" s="5"/>
+      <c r="G15" s="6" t="n">
         <f aca="false">B15*E15</f>
         <v>35</v>
       </c>
-      <c r="H15" s="3"/>
-      <c r="I15" s="5" t="n">
+      <c r="H15" s="5"/>
+      <c r="I15" s="7" t="n">
         <f aca="false">C15^B15</f>
         <v>34359738368</v>
       </c>

</xml_diff>